<commit_message>
Implemented mthcutoff 6 months
</commit_message>
<xml_diff>
--- a/appt sample for Shiny.xlsx
+++ b/appt sample for Shiny.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pan (2)" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>EEE</t>
+  </si>
+  <si>
+    <t>PSDNEW</t>
   </si>
 </sst>
 </file>
@@ -574,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,6 +1327,17 @@
         <v>42005</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="8">
+        <v>43466</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>